<commit_message>
changed order of tutorials
</commit_message>
<xml_diff>
--- a/Order_Tutorials.xlsx
+++ b/Order_Tutorials.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauvi\Dropbox\NicheModeling_Kaho\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3696F821-026F-4E30-9E31-C75CDE9DF8B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="408" windowWidth="21828" windowHeight="8220"/>
+    <workbookView xWindow="770" yWindow="410" windowWidth="21830" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Order of tutorials</t>
   </si>
@@ -52,12 +58,18 @@
   </si>
   <si>
     <t>in.el</t>
+  </si>
+  <si>
+    <t>Introduction to the tutorial</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,7 +103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -99,14 +111,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -144,9 +159,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,9 +194,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,9 +246,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -389,21 +438,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -411,7 +468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -419,7 +476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -427,39 +484,48 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -467,28 +533,34 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -497,24 +569,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified order of tutorials
</commit_message>
<xml_diff>
--- a/Order_Tutorials.xlsx
+++ b/Order_Tutorials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauvi\Dropbox\NicheModeling_Kaho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3696F821-026F-4E30-9E31-C75CDE9DF8B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22492111-7068-4358-A44C-53C50B2281A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="770" yWindow="410" windowWidth="21830" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Order of tutorials</t>
   </si>
@@ -442,7 +442,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,9 +491,6 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -502,19 +499,13 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -522,7 +513,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -530,7 +524,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated table info and format
</commit_message>
<xml_diff>
--- a/Order_Tutorials.xlsx
+++ b/Order_Tutorials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauvi\Dropbox\NicheModeling_Kaho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0932E4FE-2760-433B-941E-DFBFF151EDFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B6E690-6EA6-4002-B503-46AB542130AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="408" windowWidth="21828" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="770" yWindow="410" windowWidth="21830" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,39 +24,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
-    <t>Input Data</t>
-  </si>
-  <si>
-    <t>get.Ecoord</t>
-  </si>
-  <si>
-    <t>GEspace</t>
-  </si>
-  <si>
-    <t>e.ellipse</t>
-  </si>
-  <si>
-    <t>Mahalanobis</t>
-  </si>
-  <si>
     <t>nicheG</t>
   </si>
   <si>
-    <t>rs.inE</t>
-  </si>
-  <si>
-    <t>fitNiche</t>
-  </si>
-  <si>
     <t>get.table</t>
   </si>
   <si>
-    <t>accumulation curve</t>
-  </si>
-  <si>
-    <t>in.el</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -67,6 +40,33 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>Descriptions of initial datasets</t>
+  </si>
+  <si>
+    <t>Getting environmental values for the study sites</t>
+  </si>
+  <si>
+    <t>Plotting our datasets in G-space and E-space</t>
+  </si>
+  <si>
+    <t>Mahalanobis model</t>
+  </si>
+  <si>
+    <t>Plotting an ellipsoid in E-space</t>
+  </si>
+  <si>
+    <t>How to simulate a random sample of environmental conditions inside an region</t>
+  </si>
+  <si>
+    <t>How to identify points inside and outside the fundamental niche</t>
+  </si>
+  <si>
+    <t>Weighted-normal model</t>
+  </si>
+  <si>
+    <t>Evaluation method: accumulation curve of occurrences</t>
   </si>
 </sst>
 </file>
@@ -445,122 +445,125 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="33.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -574,7 +577,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -586,7 +589,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated titles in tutorials
</commit_message>
<xml_diff>
--- a/Order_Tutorials.xlsx
+++ b/Order_Tutorials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauvi\Dropbox\NicheModeling_Kaho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B6E690-6EA6-4002-B503-46AB542130AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65DE2DB-3FFC-426C-8E33-DBCE554B337F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="770" yWindow="410" windowWidth="21830" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>nicheG</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Evaluation method: accumulation curve of occurrences</t>
+  </si>
+  <si>
+    <t>Name of Rmd file</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,6 +462,9 @@
       </c>
       <c r="B1" t="s">
         <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>